<commit_message>
Added use of xlwings make links and file name non static
</commit_message>
<xml_diff>
--- a/invoices/Company ABC.xlsx
+++ b/invoices/Company ABC.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Excel_Examples\Expense_Report\invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E57A49C0-F160-4AF9-82FD-1E3A59EC0B32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A843186C-F852-4AC6-AF9A-CD976A785BF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="570" windowWidth="17070" windowHeight="15330" xr2:uid="{BB517DCB-9FDB-4E55-BF35-6AF19BC88A60}"/>
+    <workbookView xWindow="57480" yWindow="60" windowWidth="29040" windowHeight="15990" xr2:uid="{72A3B7CA-280D-4414-B328-C43FFFACE24B}"/>
   </bookViews>
   <sheets>
     <sheet name="Company ABC-20" sheetId="2" r:id="rId1"/>
@@ -327,7 +327,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2E32C7B-B4BD-4B56-98B2-96CAB19A0675}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64FDA051-52F2-47A2-B512-ACBDC12910D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -687,9 +687,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913C6542-5052-46F3-ADDA-546C6957DB2C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8DF27D-FC3C-4E85-8A40-B2DA4B681349}">
   <sheetPr codeName="Sheet5">
-    <tabColor theme="4" tint="0.79998168889431442"/>
+    <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:AJ84"/>
   <sheetViews>
@@ -1493,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="6">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="1"/>
@@ -4283,8 +4283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F37A97-9DFD-45F7-86CA-54B90E4799F1}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29A0410-662F-4291-BCB0-A6C063544696}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Deleted non required excel files
</commit_message>
<xml_diff>
--- a/invoices/Company ABC.xlsx
+++ b/invoices/Company ABC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Excel_Examples\Expense_Report\invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A843186C-F852-4AC6-AF9A-CD976A785BF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{955A41E5-6A70-4CD0-9F70-BF2A1C9F17D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="60" windowWidth="29040" windowHeight="15990" xr2:uid="{72A3B7CA-280D-4414-B328-C43FFFACE24B}"/>
+    <workbookView xWindow="57480" yWindow="60" windowWidth="29040" windowHeight="15990" xr2:uid="{8157B626-36AC-45A7-9742-29F3EDD7B447}"/>
   </bookViews>
   <sheets>
     <sheet name="Company ABC-20" sheetId="2" r:id="rId1"/>
@@ -327,7 +327,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64FDA051-52F2-47A2-B512-ACBDC12910D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F496DBE-AA9E-4E56-BB7C-25EFDCF94914}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -687,14 +687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8DF27D-FC3C-4E85-8A40-B2DA4B681349}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1CFAEC-3142-407D-98D8-586D54FD4E34}">
   <sheetPr codeName="Sheet5">
-    <tabColor theme="7" tint="0.59999389629810485"/>
+    <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:AJ84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="6">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="1"/>
@@ -4283,7 +4283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29A0410-662F-4291-BCB0-A6C063544696}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5024D93B-EEB3-4FAB-95BE-BF284D4BC363}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
clean up of excel files and folders
</commit_message>
<xml_diff>
--- a/invoices/Company ABC.xlsx
+++ b/invoices/Company ABC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Excel_Examples\Expense_Report\invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{955A41E5-6A70-4CD0-9F70-BF2A1C9F17D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D248D7A-0D84-43EA-AFED-CE38D45C18E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="60" windowWidth="29040" windowHeight="15990" xr2:uid="{8157B626-36AC-45A7-9742-29F3EDD7B447}"/>
+    <workbookView xWindow="29190" yWindow="570" windowWidth="21045" windowHeight="15495" xr2:uid="{77A7EDC9-20F0-4088-9331-E28818DDA45C}"/>
   </bookViews>
   <sheets>
     <sheet name="Company ABC-20" sheetId="2" r:id="rId1"/>
@@ -312,22 +312,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>53976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>97367</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F496DBE-AA9E-4E56-BB7C-25EFDCF94914}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33C88705-497A-4A09-AE3E-CE020701E13F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -349,8 +349,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="419100" y="742950"/>
-          <a:ext cx="2000250" cy="973667"/>
+          <a:off x="482600" y="911226"/>
+          <a:ext cx="2000250" cy="974725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -687,14 +687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1CFAEC-3142-407D-98D8-586D54FD4E34}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85B5450-7EA8-4753-979B-86667FB49A6D}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:AJ84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="6">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="1"/>
@@ -1577,7 +1577,7 @@
         <v>4</v>
       </c>
       <c r="J15" s="8">
-        <v>44134</v>
+        <v>44138</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="1"/>
@@ -1621,7 +1621,7 @@
         <v>6</v>
       </c>
       <c r="J16" s="9">
-        <v>44146</v>
+        <v>44150</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="1"/>
@@ -4278,12 +4278,13 @@
     <mergeCell ref="C45:J45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5024D93B-EEB3-4FAB-95BE-BF284D4BC363}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2381DCB5-DB39-482C-8499-2773E0718A0B}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>